<commit_message>
Fichier joueur.py + Fiche récap temps
</commit_message>
<xml_diff>
--- a/projet/Fiche de suivi projet python.xlsx
+++ b/projet/Fiche de suivi projet python.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="25">
   <si>
     <t xml:space="preserve">Chef de projet : Fabrice</t>
   </si>
@@ -60,6 +60,18 @@
     <t xml:space="preserve">Maël</t>
   </si>
   <si>
+    <t xml:space="preserve">Initialisation du GIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fichier joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thauvin</t>
   </si>
   <si>
@@ -73,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve">un joueur sera représenté par un dictionnaire avec comme clé le nom du joueur et comme valeur une liste d'entiers représentant les trésors du joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MàJ : Joueur : représentation par un tuple avec un str pour le nom du joueur et une liste d’entier représentant les trésor du joueur</t>
   </si>
   <si>
     <t xml:space="preserve">et enfin liste joueurs qui comme le sujet l'indique est une liste de joueurs donc dans notre cas, une liste de dictionnaires</t>
@@ -223,15 +238,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>619200</xdr:colOff>
+      <xdr:colOff>619560</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>66600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>502560</xdr:colOff>
+      <xdr:colOff>502200</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -244,8 +259,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4498920" y="1466640"/>
-          <a:ext cx="5990760" cy="4495320"/>
+          <a:off x="4699080" y="1466640"/>
+          <a:ext cx="5990400" cy="4494960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -267,14 +282,15 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,6 +381,12 @@
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B17" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="6"/>
@@ -373,13 +395,19 @@
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,7 +415,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,12 +430,12 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -419,12 +447,12 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -434,8 +462,10 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -504,7 +534,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -517,7 +547,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,10 +560,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +573,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,15 +581,15 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,7 +599,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -615,7 +645,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -628,7 +658,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,10 +671,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,7 +684,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,15 +692,15 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,7 +710,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -726,7 +756,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -739,7 +769,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,10 +782,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,7 +795,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,15 +803,15 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,7 +821,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -837,7 +867,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -850,7 +880,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,10 +893,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,7 +906,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,15 +914,15 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +932,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -929,7 +959,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -948,7 +978,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -961,7 +991,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,10 +1004,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,7 +1017,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,15 +1025,15 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1043,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>